<commit_message>
binary tree dsa craacker sheet questions started
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="476">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1439,6 +1439,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Hint</t>
   </si>
 </sst>
 </file>
@@ -1569,7 +1572,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1600,6 +1603,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -1615,6 +1621,70 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>178</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>7620</xdr:colOff>
+          <xdr:row>179</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1027"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="13639800" y="35265360"/>
+              <a:ext cx="815340" cy="205740"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1911,11 +1981,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H481"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1926,18 +1996,18 @@
     <col min="4" max="11" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1954,8 +2024,11 @@
       <c r="F4" s="12" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="12" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>470</v>
       </c>
@@ -1966,7 +2039,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1983,7 +2056,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -2000,7 +2073,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2017,7 +2090,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -2034,7 +2107,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -2051,7 +2124,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2068,7 +2141,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -2085,7 +2158,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2102,7 +2175,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -2119,7 +2192,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
@@ -2136,7 +2209,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
@@ -3867,44 +3940,68 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B176" s="7"/>
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A177" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C177" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C177" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D177" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F177" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="H177" s="13">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A178" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C178" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C178" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D178" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F178" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H178" s="13">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A179" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C179" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C179" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F179" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="H179" s="13">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A180" s="5" t="s">
         <v>172</v>
       </c>
@@ -3915,7 +4012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A181" s="5" t="s">
         <v>172</v>
       </c>
@@ -3926,7 +4023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A182" s="5" t="s">
         <v>172</v>
       </c>
@@ -3937,7 +4034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A183" s="5" t="s">
         <v>172</v>
       </c>
@@ -3948,7 +4045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A184" s="5" t="s">
         <v>172</v>
       </c>
@@ -3959,7 +4056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A185" s="5" t="s">
         <v>172</v>
       </c>
@@ -3970,7 +4067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A186" s="5" t="s">
         <v>172</v>
       </c>
@@ -3981,7 +4078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A187" s="5" t="s">
         <v>172</v>
       </c>
@@ -3992,7 +4089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A188" s="5" t="s">
         <v>172</v>
       </c>
@@ -4003,7 +4100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A189" s="5" t="s">
         <v>172</v>
       </c>
@@ -4014,7 +4111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A190" s="5" t="s">
         <v>172</v>
       </c>
@@ -4025,7 +4122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A191" s="5" t="s">
         <v>172</v>
       </c>
@@ -4036,7 +4133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A192" s="5" t="s">
         <v>172</v>
       </c>
@@ -7554,5 +7651,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId447"/>
+  <drawing r:id="rId448"/>
+  <legacyDrawing r:id="rId449"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zig zag traversal is complete
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="476">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,7 +1647,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1027"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1028"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1984,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4008,8 +4008,17 @@
       <c r="B180" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C180" s="4" t="s">
-        <v>5</v>
+      <c r="C180" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D180" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F180" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="H180" s="13">
+        <v>44262</v>
       </c>
     </row>
     <row r="181" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4019,8 +4028,17 @@
       <c r="B181" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C181" s="4" t="s">
-        <v>5</v>
+      <c r="C181" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D181" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F181" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H181" s="13">
+        <v>44262</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4030,8 +4048,17 @@
       <c r="B182" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C182" s="4" t="s">
-        <v>5</v>
+      <c r="C182" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D182" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F182" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="H182" s="13">
+        <v>44262</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4041,8 +4068,17 @@
       <c r="B183" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C183" s="4" t="s">
-        <v>5</v>
+      <c r="C183" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D183" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F183" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H183" s="13">
+        <v>44262</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4052,8 +4088,17 @@
       <c r="B184" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C184" s="4" t="s">
-        <v>5</v>
+      <c r="C184" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D184" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F184" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H184" s="13">
+        <v>44262</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4063,8 +4108,17 @@
       <c r="B185" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C185" s="4" t="s">
-        <v>5</v>
+      <c r="C185" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D185" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F185" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="H185" s="13">
+        <v>44262</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4074,8 +4128,17 @@
       <c r="B186" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C186" s="4" t="s">
-        <v>5</v>
+      <c r="C186" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D186" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F186" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H186" s="13">
+        <v>44262</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4085,8 +4148,17 @@
       <c r="B187" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C187" s="4" t="s">
-        <v>5</v>
+      <c r="C187" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D187" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F187" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="H187" s="13">
+        <v>44266</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4096,8 +4168,17 @@
       <c r="B188" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C188" s="4" t="s">
-        <v>5</v>
+      <c r="C188" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D188" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F188" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H188" s="13">
+        <v>44266</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
printing linked list in reverse order
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="476">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,7 +1647,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1028"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1036"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1984,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="B189" sqref="B189"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2602,7 +2602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="5" t="s">
         <v>43</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="5" t="s">
         <v>43</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>43</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>43</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
         <v>43</v>
       </c>
@@ -2657,35 +2657,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C56" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H56" s="13">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C57" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H57" s="13">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="5" t="s">
         <v>54</v>
       </c>
@@ -2696,7 +2714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>54</v>
       </c>
@@ -2707,7 +2725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>54</v>
       </c>
@@ -2718,7 +2736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>54</v>
       </c>
@@ -2729,7 +2747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
         <v>54</v>
       </c>
@@ -2740,7 +2758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>54</v>
       </c>
@@ -2751,7 +2769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>54</v>
       </c>
@@ -3114,7 +3132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="5" t="s">
         <v>54</v>
       </c>
@@ -3125,7 +3143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="5" t="s">
         <v>54</v>
       </c>
@@ -3136,35 +3154,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="5"/>
       <c r="B100" s="7"/>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C101" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H101" s="13">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C102" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H102" s="13">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="5" t="s">
         <v>98</v>
       </c>
@@ -3175,18 +3211,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A104" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C104" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H104" s="13">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A105" s="5" t="s">
         <v>98</v>
       </c>
@@ -3197,7 +3242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A106" s="5" t="s">
         <v>98</v>
       </c>
@@ -3208,7 +3253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="5" t="s">
         <v>98</v>
       </c>
@@ -3219,7 +3264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="5" t="s">
         <v>98</v>
       </c>
@@ -3230,7 +3275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="5" t="s">
         <v>98</v>
       </c>
@@ -3241,7 +3286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" s="5" t="s">
         <v>98</v>
       </c>
@@ -3252,7 +3297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="5" t="s">
         <v>98</v>
       </c>
@@ -3263,7 +3308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="5" t="s">
         <v>98</v>
       </c>
@@ -4188,8 +4233,17 @@
       <c r="B189" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C189" s="4" t="s">
-        <v>5</v>
+      <c r="C189" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F189" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H189" s="13">
+        <v>44267</v>
       </c>
     </row>
     <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4199,8 +4253,17 @@
       <c r="B190" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C190" s="4" t="s">
-        <v>5</v>
+      <c r="C190" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D190" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F190" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H190" s="13">
+        <v>44270</v>
       </c>
     </row>
     <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4210,8 +4273,17 @@
       <c r="B191" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C191" s="4" t="s">
-        <v>5</v>
+      <c r="C191" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D191" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F191" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H191" s="13">
+        <v>44271</v>
       </c>
     </row>
     <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
construct binary tree from string is skipped
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="477">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1442,6 +1442,9 @@
   </si>
   <si>
     <t>Hint</t>
+  </si>
+  <si>
+    <t>Skip</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1650,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1036"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1039"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1984,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4286,29 +4289,47 @@
         <v>44271</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A192" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B192" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C192" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C192" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D192" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F192" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H192" s="13">
+        <v>44273</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A193" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C193" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C193" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="D193" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="F193" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="H193" s="13">
+        <v>44273</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A194" s="5" t="s">
         <v>172</v>
       </c>
@@ -4319,7 +4340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A195" s="5" t="s">
         <v>172</v>
       </c>
@@ -4330,7 +4351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A196" s="5" t="s">
         <v>172</v>
       </c>
@@ -4341,7 +4362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A197" s="5" t="s">
         <v>172</v>
       </c>
@@ -4352,7 +4373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A198" s="5" t="s">
         <v>172</v>
       </c>
@@ -4363,7 +4384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A199" s="5" t="s">
         <v>172</v>
       </c>
@@ -4374,7 +4395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A200" s="5" t="s">
         <v>172</v>
       </c>
@@ -4385,7 +4406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A201" s="5" t="s">
         <v>172</v>
       </c>
@@ -4396,7 +4417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A202" s="5" t="s">
         <v>172</v>
       </c>
@@ -4407,7 +4428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A203" s="5" t="s">
         <v>172</v>
       </c>
@@ -4418,7 +4439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A204" s="5" t="s">
         <v>172</v>
       </c>
@@ -4429,7 +4450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A205" s="5" t="s">
         <v>172</v>
       </c>
@@ -4440,7 +4461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A206" s="5" t="s">
         <v>172</v>
       </c>
@@ -4451,7 +4472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A207" s="5" t="s">
         <v>172</v>
       </c>
@@ -4462,7 +4483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A208" s="5" t="s">
         <v>172</v>
       </c>

</xml_diff>

<commit_message>
binary to dll is completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="477">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1451,7 +1451,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1521,6 +1521,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1575,7 +1582,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1609,6 +1616,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -1650,7 +1658,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1039"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1046"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1987,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3210,8 +3218,17 @@
       <c r="B103" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>5</v>
+      <c r="C103" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H103" s="13">
+        <v>44276</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3241,8 +3258,17 @@
       <c r="B105" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C105" s="4" t="s">
-        <v>5</v>
+      <c r="C105" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H105" s="13">
+        <v>44276</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3274,8 +3300,17 @@
       <c r="B108" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C108" s="4" t="s">
-        <v>5</v>
+      <c r="C108" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H108" s="13">
+        <v>44276</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4336,15 +4371,24 @@
       <c r="B194" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C194" s="4" t="s">
-        <v>5</v>
+      <c r="C194" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D194" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F194" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H194" s="13">
+        <v>44276</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A195" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B195" s="6" t="s">
+      <c r="B195" s="17" t="s">
         <v>191</v>
       </c>
       <c r="C195" s="4" t="s">

</xml_diff>

<commit_message>
construct binary tree from inorder and pre order is completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="477">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1658,7 +1658,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1046"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1048"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1995,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="B195" sqref="B195"/>
+    <sheetView tabSelected="1" topLeftCell="C177" workbookViewId="0">
+      <selection activeCell="I194" sqref="I194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4402,8 +4402,17 @@
       <c r="B196" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C196" s="4" t="s">
-        <v>5</v>
+      <c r="C196" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D196" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F196" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H196" s="13">
+        <v>44277</v>
       </c>
     </row>
     <row r="197" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
sum tree is added
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="477">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1658,7 +1658,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1048"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1050"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1995,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C177" workbookViewId="0">
-      <selection activeCell="I194" sqref="I194"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4391,8 +4391,17 @@
       <c r="B195" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="C195" s="4" t="s">
-        <v>5</v>
+      <c r="C195" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D195" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F195" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H195" s="13">
+        <v>44277</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
is sum tree is completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="479">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1445,6 +1445,12 @@
   </si>
   <si>
     <t>Skip</t>
+  </si>
+  <si>
+    <t>need to construct tree from scratch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array sorting also required basiccally </t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1558,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1575,6 +1581,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1582,7 +1599,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1617,6 +1634,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -1658,7 +1678,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1050"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1052"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1996,7 +2016,7 @@
   <dimension ref="A1:J481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+      <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4404,7 +4424,7 @@
         <v>44277</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A196" s="5" t="s">
         <v>172</v>
       </c>
@@ -4424,26 +4444,47 @@
         <v>44277</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A197" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B197" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C197" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C197" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="D197" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="F197" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="G197" s="18" t="s">
+        <v>478</v>
+      </c>
+      <c r="H197" s="13">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A198" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B198" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C198" s="4" t="s">
-        <v>5</v>
+      <c r="C198" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D198" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F198" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H198" s="13">
+        <v>44279</v>
       </c>
     </row>
     <row r="199" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4453,11 +4494,20 @@
       <c r="B199" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C199" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C199" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D199" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F199" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H199" s="13">
+        <v>44279</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A200" s="5" t="s">
         <v>172</v>
       </c>
@@ -4468,18 +4518,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A201" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C201" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C201" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="D201" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="F201" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="G201" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="H201" s="13">
+        <v>44279</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A202" s="5" t="s">
         <v>172</v>
       </c>

</xml_diff>

<commit_message>
duplicate subtree in binary tree is completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="479">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1678,7 +1678,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1052"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1054"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2016,7 +2016,7 @@
   <dimension ref="A1:J481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="B200" sqref="B200"/>
+      <selection activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4514,8 +4514,17 @@
       <c r="B200" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C200" s="4" t="s">
-        <v>5</v>
+      <c r="C200" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D200" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F200" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H200" s="13">
+        <v>44281</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
max sum in binary tree is completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1451,6 +1451,9 @@
   </si>
   <si>
     <t xml:space="preserve">array sorting also required basiccally </t>
+  </si>
+  <si>
+    <t>till now graph is not completed</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1054"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1056"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2015,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="B206" sqref="B206"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L193" sqref="L193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4547,40 +4550,70 @@
         <v>477</v>
       </c>
       <c r="H201" s="13">
-        <v>44279</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A202" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C202" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C202" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D202" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F202" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H202" s="13">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A203" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C203" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C203" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="D203" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="F203" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="G203" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="H203" s="13">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A204" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B204" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C204" s="4" t="s">
-        <v>5</v>
+      <c r="C204" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D204" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F204" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H204" s="13">
+        <v>44281</v>
       </c>
     </row>
     <row r="205" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
dsa one started bit manipulation is started
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1056"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1061"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L193" sqref="L193"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4623,8 +4623,17 @@
       <c r="B205" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C205" s="4" t="s">
-        <v>5</v>
+      <c r="C205" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D205" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F205" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H205" s="13">
+        <v>44286</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4634,8 +4643,17 @@
       <c r="B206" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C206" s="4" t="s">
-        <v>5</v>
+      <c r="C206" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D206" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F206" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H206" s="13">
+        <v>44286</v>
       </c>
     </row>
     <row r="207" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4645,8 +4663,17 @@
       <c r="B207" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C207" s="4" t="s">
-        <v>5</v>
+      <c r="C207" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D207" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F207" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H207" s="13">
+        <v>44286</v>
       </c>
     </row>
     <row r="208" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4660,18 +4687,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A209" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B209" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C209" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C209" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D209" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F209" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H209" s="13">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A210" s="5" t="s">
         <v>172</v>
       </c>
@@ -4682,7 +4718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A211" s="5" t="s">
         <v>172</v>
       </c>
@@ -4693,17 +4729,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A212" s="5"/>
       <c r="B212" s="7"/>
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A213" s="5"/>
       <c r="B213" s="7"/>
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A214" s="5" t="s">
         <v>208</v>
       </c>
@@ -4714,7 +4750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A215" s="5" t="s">
         <v>208</v>
       </c>
@@ -4725,7 +4761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A216" s="5" t="s">
         <v>208</v>
       </c>
@@ -4736,7 +4772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A217" s="5" t="s">
         <v>208</v>
       </c>
@@ -4747,7 +4783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A218" s="5" t="s">
         <v>208</v>
       </c>
@@ -4758,7 +4794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A219" s="5" t="s">
         <v>208</v>
       </c>
@@ -4769,7 +4805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A220" s="5" t="s">
         <v>208</v>
       </c>
@@ -4780,7 +4816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A221" s="5" t="s">
         <v>208</v>
       </c>
@@ -4791,7 +4827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A222" s="5" t="s">
         <v>208</v>
       </c>
@@ -4802,7 +4838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A223" s="5" t="s">
         <v>208</v>
       </c>
@@ -4813,7 +4849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A224" s="5" t="s">
         <v>208</v>
       </c>

</xml_diff>

<commit_message>
all duplicate and isomorphic(on gfg) is completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1061"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1065"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4714,8 +4714,17 @@
       <c r="B210" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C210" s="4" t="s">
-        <v>5</v>
+      <c r="C210" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D210" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F210" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H210" s="13">
+        <v>44287</v>
       </c>
     </row>
     <row r="211" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4725,8 +4734,17 @@
       <c r="B211" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C211" s="4" t="s">
-        <v>5</v>
+      <c r="C211" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D211" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F211" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H211" s="13">
+        <v>44287</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
binary tree dsa sheet questions completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1065"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1071"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B213" sqref="B213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4683,8 +4683,18 @@
       <c r="B208" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C208" s="4" t="s">
-        <v>5</v>
+      <c r="C208" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="D208" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="E208" s="10"/>
+      <c r="F208" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="H208" s="13">
+        <v>44287</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
dsa cracker sheet bit manipulation 5 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1071"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1077"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B213" sqref="B213"/>
+    <sheetView tabSelected="1" topLeftCell="C468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H479" sqref="H479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7430,7 +7430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="465" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="465" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A465" s="5" t="s">
         <v>394</v>
       </c>
@@ -7441,7 +7441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="466" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="466" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A466" s="5" t="s">
         <v>394</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="467" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="467" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A467" s="5" t="s">
         <v>394</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="468" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="468" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A468" s="5" t="s">
         <v>394</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="469" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="469" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A469" s="5" t="s">
         <v>394</v>
       </c>
@@ -7485,49 +7485,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="470" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B470" s="7"/>
       <c r="C470" s="4"/>
     </row>
-    <row r="471" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="471" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A471" s="5"/>
       <c r="B471" s="7"/>
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="472" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A472" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B472" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="C472" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="473" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C472" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D472" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F472" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H472" s="13">
+        <v>44292</v>
+      </c>
+    </row>
+    <row r="473" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A473" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B473" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="C473" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="474" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C473" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D473" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F473" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H473" s="13">
+        <v>44292</v>
+      </c>
+    </row>
+    <row r="474" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A474" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B474" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="C474" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="475" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C474" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D474" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F474" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H474" s="13">
+        <v>44292</v>
+      </c>
+    </row>
+    <row r="475" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A475" s="5" t="s">
         <v>454</v>
       </c>
@@ -7538,29 +7565,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="476" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="476" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A476" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B476" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="C476" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C476" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D476" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F476" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H476" s="13">
+        <v>44292</v>
+      </c>
+    </row>
+    <row r="477" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A477" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B477" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="C477" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="478" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C477" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D477" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F477" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H477" s="13">
+        <v>44292</v>
+      </c>
+    </row>
+    <row r="478" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A478" s="5" t="s">
         <v>454</v>
       </c>
@@ -7571,7 +7616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="479" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="479" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A479" s="5" t="s">
         <v>454</v>
       </c>
@@ -7582,7 +7627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="480" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="480" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A480" s="5" t="s">
         <v>454</v>
       </c>

</xml_diff>

<commit_message>
bit manipulation 3 question completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1077"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1082"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2019,7 +2019,7 @@
   <dimension ref="A1:J481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H479" sqref="H479"/>
+      <selection activeCell="I475" sqref="I475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7634,19 +7634,37 @@
       <c r="B480" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="C480" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="481" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C480" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D480" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F480" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H480" s="13">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A481" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B481" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="C481" s="4" t="s">
-        <v>5</v>
+      <c r="C481" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D481" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F481" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H481" s="13">
+        <v>44293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
power set using bit is completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1082"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1083"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I475" sqref="I475"/>
+    <sheetView tabSelected="1" topLeftCell="A468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B478" sqref="B478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
bit manipulation count all bits upto n term
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1083"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1085"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2019,7 +2019,7 @@
   <dimension ref="A1:J481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B478" sqref="B478"/>
+      <selection activeCell="G481" sqref="G481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7561,8 +7561,17 @@
       <c r="B475" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="C475" s="4" t="s">
-        <v>5</v>
+      <c r="C475" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D475" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F475" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H475" s="13">
+        <v>44293</v>
       </c>
     </row>
     <row r="476" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
bit manipulation dsa cracker sheet completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1085"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1086"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2019,7 +2019,7 @@
   <dimension ref="A1:J481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G481" sqref="G481"/>
+      <selection activeCell="B484" sqref="B484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
total 10 bit manipulation questions completed on gfg
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1086"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1091"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B484" sqref="B484"/>
+    <sheetView tabSelected="1" topLeftCell="C81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2744,8 +2744,17 @@
       <c r="B58" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>5</v>
+      <c r="C58" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H58" s="13">
+        <v>44293</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2755,8 +2764,17 @@
       <c r="B59" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>5</v>
+      <c r="C59" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H59" s="13">
+        <v>44293</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -7621,8 +7639,17 @@
       <c r="B478" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="C478" s="4" t="s">
-        <v>5</v>
+      <c r="C478" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D478" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F478" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H478" s="13">
+        <v>44293</v>
       </c>
     </row>
     <row r="479" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -7632,8 +7659,17 @@
       <c r="B479" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C479" s="4" t="s">
-        <v>5</v>
+      <c r="C479" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D479" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F479" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="H479" s="13">
+        <v>44293</v>
       </c>
     </row>
     <row r="480" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
array intern 8 ques seen 2  rem
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1091"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1093"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2259,8 +2259,11 @@
       <c r="F16" s="9" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H16" s="13">
+        <v>44304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -2277,21 +2280,21 @@
         <v>466</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>467</v>
+      <c r="C18" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
DSA crackersheet Array 14 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -1681,7 +1681,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1093"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1094"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2280,7 +2280,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>6</v>
       </c>
@@ -2297,21 +2297,24 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>467</v>
+      <c r="C19" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H19" s="13">
+        <v>44327</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
DSA crackersheet Array 2 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="479">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1412,9 +1412,6 @@
   </si>
   <si>
     <t>DONE</t>
-  </si>
-  <si>
-    <t>COPY</t>
   </si>
   <si>
     <t>DONE LATER</t>
@@ -1681,7 +1678,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1094"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1097"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2018,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2052,25 +2049,25 @@
         <v>4</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2270,14 +2267,17 @@
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>466</v>
+      <c r="C17" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H17" s="13">
+        <v>44327</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2325,21 +2325,30 @@
         <v>21</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="C21" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H21" s="13">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
@@ -2347,19 +2356,19 @@
         <v>23</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>472</v>
-      </c>
       <c r="F22" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>471</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>472</v>
       </c>
       <c r="H22" s="13">
         <v>44160</v>
@@ -2711,13 +2720,13 @@
         <v>55</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H56" s="13">
         <v>44271</v>
@@ -2731,13 +2740,13 @@
         <v>56</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H57" s="13">
         <v>44271</v>
@@ -2751,13 +2760,13 @@
         <v>57</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H58" s="13">
         <v>44293</v>
@@ -2771,13 +2780,13 @@
         <v>58</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H59" s="13">
         <v>44293</v>
@@ -3226,13 +3235,13 @@
         <v>99</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H101" s="13">
         <v>44272</v>
@@ -3246,13 +3255,13 @@
         <v>100</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H102" s="13">
         <v>44272</v>
@@ -3266,13 +3275,13 @@
         <v>101</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H103" s="13">
         <v>44276</v>
@@ -3286,13 +3295,13 @@
         <v>102</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H104" s="13">
         <v>44272</v>
@@ -3306,13 +3315,13 @@
         <v>103</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H105" s="13">
         <v>44276</v>
@@ -3348,13 +3357,13 @@
         <v>106</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H108" s="13">
         <v>44276</v>
@@ -4088,7 +4097,7 @@
         <v>465</v>
       </c>
       <c r="F177" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H177" s="13">
         <v>44260</v>
@@ -4108,7 +4117,7 @@
         <v>465</v>
       </c>
       <c r="F178" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H178" s="13">
         <v>44260</v>
@@ -4125,7 +4134,7 @@
         <v>465</v>
       </c>
       <c r="F179" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H179" s="13">
         <v>44260</v>
@@ -4145,7 +4154,7 @@
         <v>465</v>
       </c>
       <c r="F180" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H180" s="13">
         <v>44262</v>
@@ -4165,7 +4174,7 @@
         <v>465</v>
       </c>
       <c r="F181" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H181" s="13">
         <v>44262</v>
@@ -4185,7 +4194,7 @@
         <v>465</v>
       </c>
       <c r="F182" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H182" s="13">
         <v>44262</v>
@@ -4205,7 +4214,7 @@
         <v>465</v>
       </c>
       <c r="F183" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H183" s="13">
         <v>44262</v>
@@ -4225,7 +4234,7 @@
         <v>465</v>
       </c>
       <c r="F184" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H184" s="13">
         <v>44262</v>
@@ -4245,7 +4254,7 @@
         <v>465</v>
       </c>
       <c r="F185" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H185" s="13">
         <v>44262</v>
@@ -4265,7 +4274,7 @@
         <v>465</v>
       </c>
       <c r="F186" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H186" s="13">
         <v>44262</v>
@@ -4285,7 +4294,7 @@
         <v>465</v>
       </c>
       <c r="F187" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H187" s="13">
         <v>44266</v>
@@ -4305,7 +4314,7 @@
         <v>465</v>
       </c>
       <c r="F188" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H188" s="13">
         <v>44266</v>
@@ -4399,13 +4408,13 @@
         <v>189</v>
       </c>
       <c r="C193" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D193" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F193" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H193" s="13">
         <v>44273</v>
@@ -4479,16 +4488,16 @@
         <v>193</v>
       </c>
       <c r="C197" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D197" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F197" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G197" s="18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H197" s="13">
         <v>44278</v>
@@ -4562,16 +4571,16 @@
         <v>197</v>
       </c>
       <c r="C201" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="D201" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="F201" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="G201" s="18" t="s">
         <v>476</v>
-      </c>
-      <c r="D201" s="11" t="s">
-        <v>476</v>
-      </c>
-      <c r="F201" s="11" t="s">
-        <v>476</v>
-      </c>
-      <c r="G201" s="18" t="s">
-        <v>477</v>
       </c>
       <c r="H201" s="13">
         <v>44281</v>
@@ -4605,16 +4614,16 @@
         <v>199</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D203" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F203" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G203" s="18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H203" s="13">
         <v>44281</v>
@@ -4708,14 +4717,14 @@
         <v>204</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D208" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E208" s="10"/>
       <c r="F208" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H208" s="13">
         <v>44287</v>
@@ -7532,7 +7541,7 @@
         <v>465</v>
       </c>
       <c r="F472" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H472" s="13">
         <v>44292</v>
@@ -7552,7 +7561,7 @@
         <v>465</v>
       </c>
       <c r="F473" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H473" s="13">
         <v>44292</v>
@@ -7572,7 +7581,7 @@
         <v>465</v>
       </c>
       <c r="F474" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H474" s="13">
         <v>44292</v>
@@ -7592,7 +7601,7 @@
         <v>465</v>
       </c>
       <c r="F475" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H475" s="13">
         <v>44293</v>
@@ -7612,7 +7621,7 @@
         <v>465</v>
       </c>
       <c r="F476" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H476" s="13">
         <v>44292</v>
@@ -7632,7 +7641,7 @@
         <v>465</v>
       </c>
       <c r="F477" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H477" s="13">
         <v>44292</v>
@@ -7652,7 +7661,7 @@
         <v>465</v>
       </c>
       <c r="F478" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H478" s="13">
         <v>44293</v>
@@ -7672,7 +7681,7 @@
         <v>465</v>
       </c>
       <c r="F479" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H479" s="13">
         <v>44293</v>
@@ -7692,7 +7701,7 @@
         <v>465</v>
       </c>
       <c r="F480" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H480" s="13">
         <v>44293</v>
@@ -7712,7 +7721,7 @@
         <v>465</v>
       </c>
       <c r="F481" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H481" s="13">
         <v>44293</v>

</xml_diff>

<commit_message>
DSA crackersheet Array 3 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="479">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1678,7 +1678,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1097"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1104"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2015,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2381,8 +2381,17 @@
       <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>5</v>
+      <c r="C23" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H23" s="13">
+        <v>44327</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2403,8 +2412,17 @@
       <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>5</v>
+      <c r="C25" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H25" s="13">
+        <v>44328</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2414,8 +2432,17 @@
       <c r="B26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>5</v>
+      <c r="C26" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H26" s="13">
+        <v>44328</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
codechef contest may 2021 2 question solved
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -1678,7 +1678,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1104"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1105"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2015,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
DSA crackersheet Array 1 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1108"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1110"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,11 +2474,11 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
@@ -2499,11 +2499,11 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
@@ -2515,11 +2515,11 @@
       <c r="C24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2603,14 +2603,23 @@
       <c r="B28" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
+      <c r="C28" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H28" s="13">
+        <v>44330</v>
+      </c>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2631,13 +2640,13 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
@@ -2646,14 +2655,23 @@
       <c r="B30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
+      <c r="C30" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H30" s="13">
+        <v>44330</v>
+      </c>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
@@ -2665,11 +2683,11 @@
       <c r="C31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -2681,11 +2699,11 @@
       <c r="C32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
@@ -7932,6 +7950,24 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="J21:N21"/>
     <mergeCell ref="J29:N29"/>
     <mergeCell ref="J30:N30"/>
     <mergeCell ref="J31:N31"/>
@@ -7942,24 +7978,6 @@
     <mergeCell ref="J26:N26"/>
     <mergeCell ref="J27:N27"/>
     <mergeCell ref="J28:N28"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="J10:N10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
DSA crackersheet Array 4 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1110"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1113"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2032,7 +2032,7 @@
   <dimension ref="A1:N481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,11 +2474,11 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
@@ -2499,11 +2499,11 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
@@ -2515,11 +2515,11 @@
       <c r="C24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2615,11 +2615,11 @@
       <c r="H28" s="13">
         <v>44330</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2640,13 +2640,13 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
@@ -2667,11 +2667,11 @@
       <c r="H30" s="13">
         <v>44330</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
@@ -2683,11 +2683,11 @@
       <c r="C31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -2696,49 +2696,85 @@
       <c r="B32" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C32" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H32" s="13">
+        <v>44332</v>
+      </c>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C33" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H33" s="13">
+        <v>44332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C34" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H34" s="13">
+        <v>44332</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H35" s="13">
+        <v>44332</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -2749,7 +2785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
@@ -2760,7 +2796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
         <v>6</v>
       </c>
@@ -2771,7 +2807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>6</v>
       </c>
@@ -2782,7 +2818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
         <v>6</v>
       </c>
@@ -2793,7 +2829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="5" t="s">
         <v>6</v>
       </c>
@@ -2804,20 +2840,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="7"/>
       <c r="C42" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
         <v>43</v>
       </c>
@@ -2828,7 +2864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
@@ -2839,7 +2875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
         <v>43</v>
       </c>
@@ -2850,7 +2886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
@@ -2861,7 +2897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
         <v>43</v>
       </c>
@@ -7950,12 +7986,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="J28:N28"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="J12:N12"/>
@@ -7968,16 +8008,12 @@
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
DSA crackersheet All  Array 32  que completed and 4 in do later section
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1123"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1132"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,13 +2474,13 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
@@ -2499,29 +2499,29 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C24" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2615,11 +2615,11 @@
       <c r="H28" s="13">
         <v>44330</v>
       </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2640,15 +2640,15 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-    </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
@@ -2667,29 +2667,29 @@
       <c r="H30" s="13">
         <v>44330</v>
       </c>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C31" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>6</v>
       </c>
@@ -2708,11 +2708,11 @@
       <c r="H32" s="13">
         <v>44332</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
@@ -2794,7 +2794,7 @@
         <v>44333</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
@@ -2814,26 +2814,35 @@
         <v>44333</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="11" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>5</v>
+      <c r="C39" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H39" s="13">
+        <v>44333</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2896,8 +2905,17 @@
       <c r="B44" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>5</v>
+      <c r="C44" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H44" s="13">
+        <v>44334</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2907,8 +2925,17 @@
       <c r="B45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>5</v>
+      <c r="C45" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H45" s="13">
+        <v>44334</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3600,7 +3627,7 @@
         <v>44272</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A105" s="5" t="s">
         <v>98</v>
       </c>
@@ -3620,29 +3647,29 @@
         <v>44276</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A106" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C106" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C106" s="11" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A107" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C107" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C107" s="11" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A108" s="5" t="s">
         <v>98</v>
       </c>
@@ -8022,16 +8049,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="J12:N12"/>
@@ -8044,12 +8067,16 @@
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="J28:N28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
DSA crackersheet 2D  Array 2 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1132"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1133"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,11 +2474,11 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
@@ -2499,11 +2499,11 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
@@ -2515,11 +2515,11 @@
       <c r="C24" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2615,11 +2615,11 @@
       <c r="H28" s="13">
         <v>44330</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2640,13 +2640,13 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
@@ -2667,11 +2667,11 @@
       <c r="H30" s="13">
         <v>44330</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
@@ -2683,11 +2683,11 @@
       <c r="C31" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -2708,11 +2708,11 @@
       <c r="H32" s="13">
         <v>44332</v>
       </c>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
@@ -8049,12 +8049,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="J28:N28"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="J12:N12"/>
@@ -8067,16 +8071,12 @@
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
DSA crackersheet 2D  Array 1 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1133"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1136"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31:N31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,11 +2474,11 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
@@ -2499,11 +2499,11 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
@@ -2515,11 +2515,11 @@
       <c r="C24" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2615,11 +2615,11 @@
       <c r="H28" s="13">
         <v>44330</v>
       </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2640,13 +2640,13 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
@@ -2667,11 +2667,11 @@
       <c r="H30" s="13">
         <v>44330</v>
       </c>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
@@ -2683,11 +2683,11 @@
       <c r="C31" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -2708,11 +2708,11 @@
       <c r="H32" s="13">
         <v>44332</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
@@ -2945,8 +2945,17 @@
       <c r="B46" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>5</v>
+      <c r="C46" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H46" s="13">
+        <v>44336</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -8049,16 +8058,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="J12:N12"/>
@@ -8071,12 +8076,16 @@
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="J28:N28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
codechef dsa learing 3 questions solved
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1139"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1146"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,11 +2474,11 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
@@ -2499,11 +2499,11 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
@@ -2515,11 +2515,11 @@
       <c r="C24" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2615,11 +2615,11 @@
       <c r="H28" s="13">
         <v>44330</v>
       </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2640,13 +2640,13 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
@@ -2667,11 +2667,11 @@
       <c r="H30" s="13">
         <v>44330</v>
       </c>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
@@ -2683,11 +2683,11 @@
       <c r="C31" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -2708,11 +2708,11 @@
       <c r="H32" s="13">
         <v>44332</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
@@ -2985,8 +2985,17 @@
       <c r="B48" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>5</v>
+      <c r="C48" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H48" s="13">
+        <v>44337</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -8067,16 +8076,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="J12:N12"/>
@@ -8089,12 +8094,16 @@
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="J28:N28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
DSA crackersheet 2D  Array 3 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1146"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1153"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,11 +2474,11 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
@@ -2499,11 +2499,11 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
@@ -2515,11 +2515,11 @@
       <c r="C24" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2615,11 +2615,11 @@
       <c r="H28" s="13">
         <v>44330</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2640,13 +2640,13 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
@@ -2667,11 +2667,11 @@
       <c r="H30" s="13">
         <v>44330</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
@@ -2683,11 +2683,11 @@
       <c r="C31" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -2708,11 +2708,11 @@
       <c r="H32" s="13">
         <v>44332</v>
       </c>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
@@ -3005,8 +3005,17 @@
       <c r="B49" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>5</v>
+      <c r="C49" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H49" s="13">
+        <v>44339</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3027,8 +3036,17 @@
       <c r="B51" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>5</v>
+      <c r="C51" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H51" s="13">
+        <v>44339</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -3049,8 +3067,17 @@
       <c r="B53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>5</v>
+      <c r="C53" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H53" s="13">
+        <v>44339</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8076,12 +8103,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="J28:N28"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="J12:N12"/>
@@ -8094,16 +8125,12 @@
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
DSA crackersheet ALL 2D  Array 10 que completed
</commit_message>
<xml_diff>
--- a/DSA crack sheet/File.xlsx
+++ b/DSA crack sheet/File.xlsx
@@ -1647,11 +1647,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1694,7 +1694,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1157"/>
+                  <a14:cameraTool cellRange="$D$177" spid="_x0000_s1159"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A461" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N476" sqref="N476"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2085,11 +2085,11 @@
       <c r="H5" t="s">
         <v>473</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
@@ -2107,11 +2107,11 @@
       <c r="F6" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
@@ -2129,11 +2129,11 @@
       <c r="F7" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
@@ -2151,11 +2151,11 @@
       <c r="F8" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2173,11 +2173,11 @@
       <c r="F9" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
@@ -2195,11 +2195,11 @@
       <c r="F10" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2217,11 +2217,11 @@
       <c r="F11" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
@@ -2239,11 +2239,11 @@
       <c r="F12" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -2261,11 +2261,11 @@
       <c r="F13" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -2283,11 +2283,11 @@
       <c r="F14" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -2305,11 +2305,11 @@
       <c r="F15" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -2330,11 +2330,11 @@
       <c r="H16" s="13">
         <v>44304</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -2355,11 +2355,11 @@
       <c r="H17" s="13">
         <v>44327</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
@@ -2377,11 +2377,11 @@
       <c r="F18" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
@@ -2402,11 +2402,11 @@
       <c r="H19" s="13">
         <v>44327</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
@@ -2418,11 +2418,11 @@
       <c r="C20" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
@@ -2443,11 +2443,11 @@
       <c r="H21" s="13">
         <v>44327</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
@@ -2474,11 +2474,11 @@
       <c r="H22" s="13">
         <v>44160</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
@@ -2499,11 +2499,11 @@
       <c r="H23" s="13">
         <v>44327</v>
       </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
@@ -2515,11 +2515,11 @@
       <c r="C24" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H25" s="13">
         <v>44328</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -2565,11 +2565,11 @@
       <c r="H26" s="13">
         <v>44328</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -2590,11 +2590,11 @@
       <c r="H27" s="13">
         <v>44330</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -2615,11 +2615,11 @@
       <c r="H28" s="13">
         <v>44330</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -2640,13 +2640,13 @@
       <c r="H29" s="13">
         <v>44330</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
@@ -2667,11 +2667,11 @@
       <c r="H30" s="13">
         <v>44330</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
@@ -2683,11 +2683,11 @@
       <c r="C31" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -2708,11 +2708,11 @@
       <c r="H32" s="13">
         <v>44332</v>
       </c>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
@@ -8121,12 +8121,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="J28:N28"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="J12:N12"/>
@@ -8139,16 +8143,12 @@
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="J21:N21"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J9:N9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>